<commit_message>
Updated checklist for test automation
</commit_message>
<xml_diff>
--- a/sharelane_checklist.xlsx
+++ b/sharelane_checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Test Automation\Java\hw4_Sharelane\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Test Automation\Java\hw4_Sharelane\hw4_sharelane\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A263E09-D73C-42DE-9C5D-6DC419ECFB9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4C34E5C-DFEC-48B3-808E-4ADCFC74BEFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="168">
   <si>
     <t>Статус</t>
   </si>
@@ -523,7 +523,28 @@
     <t>Security вопрос: приоритет повышен</t>
   </si>
   <si>
-    <t>Секьюрити штука, поэтому Smoke</t>
+    <t>Сделано</t>
+  </si>
+  <si>
+    <t>Проверить что пароль в поле Password заменяется звёздочками при вводе</t>
+  </si>
+  <si>
+    <t>Секьюрити штука, поэтому  может быть и Smoke</t>
+  </si>
+  <si>
+    <t>Проверить что у книги есть имя и автор</t>
+  </si>
+  <si>
+    <t>Проверить что у книги есть цена, и она равна 10$</t>
+  </si>
+  <si>
+    <t>Слишком сложно, откладываю</t>
+  </si>
+  <si>
+    <t>Не делаем</t>
+  </si>
+  <si>
+    <t>Проверить что кнопка Proceed to Checkout ведёт на страницу Checkout</t>
   </si>
 </sst>
 </file>
@@ -581,7 +602,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -597,6 +618,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -653,7 +680,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -693,13 +720,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -711,15 +732,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -759,6 +778,22 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -783,19 +818,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <border>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -810,20 +832,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FE89EFD3-F5E6-427A-A4AE-782233C9841D}" name="Table1" displayName="Table1" ref="A1:J41" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FE89EFD3-F5E6-427A-A4AE-782233C9841D}" name="Table1" displayName="Table1" ref="A1:J41" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7">
   <autoFilter ref="A1:J41" xr:uid="{FE89EFD3-F5E6-427A-A4AE-782233C9841D}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{EE3982AD-7A22-45A0-95C4-92DB6AD6D684}" name="Модуль"/>
     <tableColumn id="2" xr3:uid="{81FD0C2A-A01C-4D70-98AA-1B0D68AB41BE}" name="Требование"/>
-    <tableColumn id="3" xr3:uid="{877BDE58-2F7D-494A-8CF6-06C84230D253}" name="Тест-кейс" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{6E661433-9F32-4310-B633-8437D100F54A}" name="Тип теста" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{877BDE58-2F7D-494A-8CF6-06C84230D253}" name="Тест-кейс" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{6E661433-9F32-4310-B633-8437D100F54A}" name="Тип теста" dataDxfId="5"/>
     <tableColumn id="5" xr3:uid="{033B4E9F-E3B9-4C5C-B93C-AE9F832D011E}" name="Сложность (5 = легко)"/>
     <tableColumn id="6" xr3:uid="{3EC32434-BCAA-4BAD-A4EB-C9E61CDCC1FF}" name="Критичность (технологии)"/>
     <tableColumn id="7" xr3:uid="{EDCB3ACD-4F2E-40F0-B526-D7C7ED84AAF3}" name="Критичность (бизнес)"/>
     <tableColumn id="8" xr3:uid="{791AC5C8-1A31-4981-8DA5-4201C560ED4A}" name="Приоритет">
       <calculatedColumnFormula>SUM(E2:G2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{BD715C9F-58F7-4910-B6B9-524C0EC87A85}" name="Статус" dataDxfId="0">
+    <tableColumn id="9" xr3:uid="{BD715C9F-58F7-4910-B6B9-524C0EC87A85}" name="Статус" dataDxfId="4">
       <calculatedColumnFormula>Table13[[#This Row],[Статус]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{D11A28CE-55DC-4CF9-96AB-4EA552A5C688}" name="Комментарии"/>
@@ -833,15 +855,21 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6998AABF-FC77-48A5-8AA0-30BE1579D29E}" name="Table13" displayName="Table13" ref="A1:F41" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3">
-  <autoFilter ref="A1:F41" xr:uid="{FE89EFD3-F5E6-427A-A4AE-782233C9841D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6998AABF-FC77-48A5-8AA0-30BE1579D29E}" name="Table13" displayName="Table13" ref="A1:F41" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2">
+  <autoFilter ref="A1:F41" xr:uid="{FE89EFD3-F5E6-427A-A4AE-782233C9841D}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Делаем"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F41">
     <sortCondition descending="1" ref="D1:D41"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{D5D7C9F8-4B1F-412C-8FF2-6F8DC0F54C75}" name="Модуль"/>
-    <tableColumn id="3" xr3:uid="{F9A68072-5A64-4BB2-9A67-2824EE1D1EDF}" name="Тест-кейс" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{7081D3CF-0355-45A9-BF8E-AAF1ACAAF437}" name="Тип теста" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{F9A68072-5A64-4BB2-9A67-2824EE1D1EDF}" name="Тест-кейс" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{7081D3CF-0355-45A9-BF8E-AAF1ACAAF437}" name="Тип теста" dataDxfId="0"/>
     <tableColumn id="8" xr3:uid="{273AD8A4-80D7-40E4-94EA-A0BCF69349F1}" name="Приоритет">
       <calculatedColumnFormula>SUM(#REF!)</calculatedColumnFormula>
     </tableColumn>
@@ -1117,7 +1145,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF2C0FFA-4AC8-4261-BB0E-4C3B659E1E3D}">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A27" workbookViewId="0">
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
@@ -1247,7 +1275,7 @@
       <c r="A10" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="15" t="s">
         <v>49</v>
       </c>
       <c r="C10" s="7" t="s">
@@ -1266,7 +1294,7 @@
       <c r="A11" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="15" t="s">
         <v>53</v>
       </c>
       <c r="C11" s="7" t="s">
@@ -1285,7 +1313,7 @@
       <c r="A12" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="15" t="s">
         <v>56</v>
       </c>
       <c r="C12" s="7" t="s">
@@ -1304,7 +1332,7 @@
       <c r="A13" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="15" t="s">
         <v>59</v>
       </c>
       <c r="C13" s="7" t="s">
@@ -1323,7 +1351,7 @@
       <c r="A14" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="15" t="s">
         <v>62</v>
       </c>
       <c r="C14" s="7" t="s">
@@ -1359,7 +1387,7 @@
       <c r="A16" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="15" t="s">
         <v>67</v>
       </c>
       <c r="C16" s="7" t="s">
@@ -1395,7 +1423,7 @@
       <c r="A18" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="15" t="s">
         <v>39</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1431,7 +1459,7 @@
       <c r="A20" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="15" t="s">
         <v>77</v>
       </c>
       <c r="C20" s="7" t="s">
@@ -1450,7 +1478,7 @@
       <c r="A21" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="15" t="s">
         <v>80</v>
       </c>
       <c r="C21" s="7" t="s">
@@ -1469,7 +1497,7 @@
       <c r="A22" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="15" t="s">
         <v>82</v>
       </c>
       <c r="C22" s="7" t="s">
@@ -1505,7 +1533,7 @@
       <c r="A24" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="15" t="s">
         <v>87</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -1524,7 +1552,7 @@
       <c r="A25" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="15" t="s">
         <v>90</v>
       </c>
       <c r="C25" s="7" t="s">
@@ -1543,7 +1571,7 @@
       <c r="A26" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="15" t="s">
         <v>93</v>
       </c>
       <c r="C26" s="7" t="s">
@@ -1579,7 +1607,7 @@
       <c r="A28" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="15" t="s">
         <v>98</v>
       </c>
       <c r="C28" s="7" t="s">
@@ -1598,7 +1626,7 @@
       <c r="A29" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="B29" s="16" t="s">
+      <c r="B29" s="15" t="s">
         <v>101</v>
       </c>
       <c r="C29" s="7" t="s">
@@ -1613,7 +1641,7 @@
       <c r="A30" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="15" t="s">
         <v>103</v>
       </c>
       <c r="C30" s="7" t="s">
@@ -1632,7 +1660,7 @@
       <c r="A31" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="15" t="s">
         <v>106</v>
       </c>
       <c r="C31" s="7" t="s">
@@ -1651,7 +1679,7 @@
       <c r="A32" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="15" t="s">
         <v>108</v>
       </c>
       <c r="C32" s="7" t="s">
@@ -1824,7 +1852,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J123"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B7" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -1843,34 +1871,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="19" t="s">
+      <c r="J1" s="17" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1902,7 +1930,7 @@
       </c>
       <c r="I2" t="str">
         <f>Table13[[#This Row],[Статус]]</f>
-        <v>Делаем</v>
+        <v>Сделано</v>
       </c>
       <c r="J2" t="s">
         <v>32</v>
@@ -1931,7 +1959,7 @@
       </c>
       <c r="I3" t="str">
         <f>Table13[[#This Row],[Статус]]</f>
-        <v>Делаем</v>
+        <v>Не делаем</v>
       </c>
       <c r="J3"/>
     </row>
@@ -1958,7 +1986,7 @@
       </c>
       <c r="I4" t="str">
         <f>Table13[[#This Row],[Статус]]</f>
-        <v>Делаем</v>
+        <v>Сделано</v>
       </c>
       <c r="J4"/>
     </row>
@@ -1985,7 +2013,7 @@
       </c>
       <c r="I5" t="str">
         <f>Table13[[#This Row],[Статус]]</f>
-        <v>Делаем</v>
+        <v>Сделано</v>
       </c>
       <c r="J5"/>
     </row>
@@ -2017,12 +2045,12 @@
       </c>
       <c r="I6" t="str">
         <f>Table13[[#This Row],[Статус]]</f>
-        <v>Делаем</v>
+        <v>Сделано</v>
       </c>
       <c r="J6"/>
     </row>
     <row r="7" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="B7" s="15"/>
+      <c r="B7" s="14"/>
       <c r="C7" s="3" t="s">
         <v>113</v>
       </c>
@@ -2044,12 +2072,12 @@
       </c>
       <c r="I7" t="str">
         <f>Table13[[#This Row],[Статус]]</f>
-        <v>Делаем</v>
+        <v>Сделано</v>
       </c>
       <c r="J7"/>
     </row>
     <row r="8" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="15"/>
+      <c r="B8" s="14"/>
       <c r="C8" s="3" t="s">
         <v>114</v>
       </c>
@@ -2071,7 +2099,7 @@
       </c>
       <c r="I8" t="str">
         <f>Table13[[#This Row],[Статус]]</f>
-        <v>Делаем</v>
+        <v>Сделано</v>
       </c>
       <c r="J8"/>
     </row>
@@ -2100,12 +2128,12 @@
       </c>
       <c r="I9" t="str">
         <f>Table13[[#This Row],[Статус]]</f>
-        <v>Делаем</v>
+        <v>Сделано</v>
       </c>
       <c r="J9"/>
     </row>
     <row r="10" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="B10" s="15"/>
+      <c r="B10" s="14"/>
       <c r="C10" s="3" t="s">
         <v>152</v>
       </c>
@@ -2127,12 +2155,12 @@
       </c>
       <c r="I10" t="str">
         <f>Table13[[#This Row],[Статус]]</f>
-        <v>Делаем</v>
+        <v>Сделано</v>
       </c>
       <c r="J10"/>
     </row>
     <row r="11" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="15"/>
+      <c r="B11" s="14"/>
       <c r="C11" s="3" t="s">
         <v>120</v>
       </c>
@@ -2154,7 +2182,7 @@
       </c>
       <c r="I11" t="str">
         <f>Table13[[#This Row],[Статус]]</f>
-        <v>Делаем</v>
+        <v>Сделано</v>
       </c>
       <c r="J11"/>
     </row>
@@ -2183,7 +2211,7 @@
       </c>
       <c r="I12" t="str">
         <f>Table13[[#This Row],[Статус]]</f>
-        <v>Делаем</v>
+        <v>Сделано</v>
       </c>
       <c r="J12"/>
     </row>
@@ -2212,12 +2240,12 @@
       </c>
       <c r="I13" t="str">
         <f>Table13[[#This Row],[Статус]]</f>
-        <v>Делаем</v>
+        <v>Сделано</v>
       </c>
       <c r="J13"/>
     </row>
     <row r="14" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="B14" s="15"/>
+      <c r="B14" s="14"/>
       <c r="C14" s="3" t="s">
         <v>118</v>
       </c>
@@ -2239,12 +2267,12 @@
       </c>
       <c r="I14" t="str">
         <f>Table13[[#This Row],[Статус]]</f>
-        <v>Делаем</v>
+        <v>Сделано</v>
       </c>
       <c r="J14"/>
     </row>
     <row r="15" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="B15" s="15"/>
+      <c r="B15" s="14"/>
       <c r="C15" s="3" t="s">
         <v>119</v>
       </c>
@@ -2266,12 +2294,12 @@
       </c>
       <c r="I15" t="str">
         <f>Table13[[#This Row],[Статус]]</f>
-        <v>Делаем</v>
+        <v>Сделано</v>
       </c>
       <c r="J15"/>
     </row>
     <row r="16" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="15"/>
+      <c r="B16" s="14"/>
       <c r="C16" s="3" t="s">
         <v>124</v>
       </c>
@@ -2293,7 +2321,7 @@
       </c>
       <c r="I16" t="str">
         <f>Table13[[#This Row],[Статус]]</f>
-        <v>Делаем</v>
+        <v>Сделано</v>
       </c>
       <c r="J16"/>
     </row>
@@ -2322,12 +2350,12 @@
       </c>
       <c r="I17" t="str">
         <f>Table13[[#This Row],[Статус]]</f>
-        <v>Делаем</v>
+        <v>Сделано</v>
       </c>
       <c r="J17"/>
     </row>
     <row r="18" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="B18" s="15"/>
+      <c r="B18" s="14"/>
       <c r="C18" s="3" t="s">
         <v>127</v>
       </c>
@@ -2349,12 +2377,12 @@
       </c>
       <c r="I18" t="str">
         <f>Table13[[#This Row],[Статус]]</f>
-        <v>Делаем</v>
+        <v>Сделано</v>
       </c>
       <c r="J18"/>
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="15"/>
+      <c r="B19" s="14"/>
       <c r="C19" s="3" t="s">
         <v>126</v>
       </c>
@@ -2376,7 +2404,7 @@
       </c>
       <c r="I19" t="str">
         <f>Table13[[#This Row],[Статус]]</f>
-        <v>Делаем</v>
+        <v>Сделано</v>
       </c>
       <c r="J19"/>
     </row>
@@ -2408,12 +2436,12 @@
       </c>
       <c r="I20" t="str">
         <f>Table13[[#This Row],[Статус]]</f>
-        <v>Делаем</v>
+        <v>Сделано</v>
       </c>
       <c r="J20"/>
     </row>
     <row r="21" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="B21" s="15"/>
+      <c r="B21" s="14"/>
       <c r="C21" s="3" t="s">
         <v>129</v>
       </c>
@@ -2435,12 +2463,12 @@
       </c>
       <c r="I21" t="str">
         <f>Table13[[#This Row],[Статус]]</f>
-        <v>Делаем</v>
+        <v>Сделано</v>
       </c>
       <c r="J21"/>
     </row>
     <row r="22" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="15"/>
+      <c r="B22" s="14"/>
       <c r="C22" s="3" t="s">
         <v>130</v>
       </c>
@@ -2462,7 +2490,7 @@
       </c>
       <c r="I22" t="str">
         <f>Table13[[#This Row],[Статус]]</f>
-        <v>Делаем</v>
+        <v>Сделано</v>
       </c>
       <c r="J22"/>
     </row>
@@ -2499,7 +2527,7 @@
       <c r="J23"/>
     </row>
     <row r="24" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="B24" s="15"/>
+      <c r="B24" s="14"/>
       <c r="C24" s="3" t="s">
         <v>133</v>
       </c>
@@ -2521,12 +2549,12 @@
       </c>
       <c r="I24" t="str">
         <f>Table13[[#This Row],[Статус]]</f>
-        <v>Делаем</v>
+        <v>Сделано</v>
       </c>
       <c r="J24"/>
     </row>
     <row r="25" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="15"/>
+      <c r="B25" s="14"/>
       <c r="C25" s="3" t="s">
         <v>134</v>
       </c>
@@ -2548,7 +2576,7 @@
       </c>
       <c r="I25" t="str">
         <f>Table13[[#This Row],[Статус]]</f>
-        <v>Делаем</v>
+        <v>Сделано</v>
       </c>
       <c r="J25"/>
     </row>
@@ -2580,12 +2608,12 @@
       </c>
       <c r="I26" t="str">
         <f>Table13[[#This Row],[Статус]]</f>
-        <v>Делаем</v>
+        <v>Сделано</v>
       </c>
       <c r="J26"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B27" s="15"/>
+      <c r="B27" s="14"/>
       <c r="C27" s="3" t="s">
         <v>136</v>
       </c>
@@ -2612,7 +2640,7 @@
       <c r="J27"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B28" s="15"/>
+      <c r="B28" s="14"/>
       <c r="C28" s="3" t="s">
         <v>137</v>
       </c>
@@ -2639,7 +2667,7 @@
       <c r="J28"/>
     </row>
     <row r="29" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="14" t="s">
         <v>101</v>
       </c>
       <c r="C29" s="3" t="s">
@@ -2729,7 +2757,7 @@
       <c r="J31"/>
     </row>
     <row r="32" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="7" t="s">
         <v>90</v>
       </c>
       <c r="C32" s="3" t="s">
@@ -2758,7 +2786,7 @@
       <c r="J32"/>
     </row>
     <row r="33" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B33" s="17" t="s">
+      <c r="B33" s="7" t="s">
         <v>98</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -3482,7 +3510,7 @@
   <dimension ref="A1:F123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3496,26 +3524,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="17" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -3528,14 +3556,14 @@
       <c r="D2">
         <v>801</v>
       </c>
-      <c r="E2" t="s">
-        <v>158</v>
+      <c r="E2" s="19" t="s">
+        <v>160</v>
       </c>
       <c r="F2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -3549,9 +3577,11 @@
         <v>800</v>
       </c>
       <c r="E3" t="s">
-        <v>158</v>
-      </c>
-      <c r="F3"/>
+        <v>166</v>
+      </c>
+      <c r="F3" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -3567,7 +3597,7 @@
         <v>800</v>
       </c>
       <c r="E4" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="F4"/>
     </row>
@@ -3585,7 +3615,7 @@
         <v>800</v>
       </c>
       <c r="E5" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="F5"/>
     </row>
@@ -3603,7 +3633,7 @@
         <v>800</v>
       </c>
       <c r="E6" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="F6"/>
     </row>
@@ -3621,7 +3651,7 @@
         <v>800</v>
       </c>
       <c r="E7" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="F7" t="s">
         <v>159</v>
@@ -3641,7 +3671,7 @@
         <v>800</v>
       </c>
       <c r="E8" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="F8" t="s">
         <v>159</v>
@@ -3661,13 +3691,13 @@
         <v>800</v>
       </c>
       <c r="E9" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="F9" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -3680,12 +3710,11 @@
       <c r="D10">
         <v>15</v>
       </c>
-      <c r="E10" t="s">
-        <v>158</v>
-      </c>
-      <c r="F10"/>
-    </row>
-    <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="E10" s="19" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -3698,12 +3727,11 @@
       <c r="D11">
         <v>15</v>
       </c>
-      <c r="E11" t="s">
-        <v>158</v>
-      </c>
-      <c r="F11"/>
-    </row>
-    <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="E11" s="19" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -3716,12 +3744,11 @@
       <c r="D12">
         <v>15</v>
       </c>
-      <c r="E12" t="s">
-        <v>158</v>
-      </c>
-      <c r="F12"/>
-    </row>
-    <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="E12" s="19" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -3734,12 +3761,11 @@
       <c r="D13">
         <v>15</v>
       </c>
-      <c r="E13" t="s">
-        <v>158</v>
-      </c>
-      <c r="F13"/>
-    </row>
-    <row r="14" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="E13" s="19" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -3752,17 +3778,17 @@
       <c r="D14">
         <v>15</v>
       </c>
-      <c r="E14" t="s">
-        <v>158</v>
+      <c r="E14" s="19" t="s">
+        <v>160</v>
       </c>
       <c r="F14"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>36</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>136</v>
+        <v>163</v>
       </c>
       <c r="C15" t="s">
         <v>122</v>
@@ -3770,17 +3796,17 @@
       <c r="D15">
         <v>15</v>
       </c>
-      <c r="E15" t="s">
-        <v>158</v>
+      <c r="E15" s="19" t="s">
+        <v>160</v>
       </c>
       <c r="F15"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>36</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>137</v>
+        <v>164</v>
       </c>
       <c r="C16" t="s">
         <v>122</v>
@@ -3788,12 +3814,12 @@
       <c r="D16">
         <v>15</v>
       </c>
-      <c r="E16" t="s">
-        <v>158</v>
+      <c r="E16" s="19" t="s">
+        <v>160</v>
       </c>
       <c r="F16"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -3806,12 +3832,12 @@
       <c r="D17">
         <v>15</v>
       </c>
-      <c r="E17" t="s">
-        <v>158</v>
+      <c r="E17" s="19" t="s">
+        <v>160</v>
       </c>
       <c r="F17"/>
     </row>
-    <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -3825,16 +3851,16 @@
         <v>15</v>
       </c>
       <c r="E18" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="F18"/>
     </row>
-    <row r="19" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>33</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>142</v>
+        <v>167</v>
       </c>
       <c r="C19" t="s">
         <v>122</v>
@@ -3843,7 +3869,7 @@
         <v>15</v>
       </c>
       <c r="E19" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="F19"/>
     </row>
@@ -3861,11 +3887,11 @@
         <v>15</v>
       </c>
       <c r="E20" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="F20"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -3878,12 +3904,12 @@
       <c r="D21">
         <v>14</v>
       </c>
-      <c r="E21" t="s">
-        <v>158</v>
+      <c r="E21" s="19" t="s">
+        <v>160</v>
       </c>
       <c r="F21"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -3896,8 +3922,8 @@
       <c r="D22">
         <v>14</v>
       </c>
-      <c r="E22" t="s">
-        <v>158</v>
+      <c r="E22" s="19" t="s">
+        <v>160</v>
       </c>
       <c r="F22"/>
     </row>
@@ -3919,7 +3945,7 @@
       </c>
       <c r="F23"/>
     </row>
-    <row r="24" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -3932,12 +3958,12 @@
       <c r="D24">
         <v>14</v>
       </c>
-      <c r="E24" t="s">
-        <v>158</v>
+      <c r="E24" s="19" t="s">
+        <v>160</v>
       </c>
       <c r="F24"/>
     </row>
-    <row r="25" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -3951,31 +3977,31 @@
         <v>14</v>
       </c>
       <c r="E25" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="F25"/>
     </row>
-    <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>30</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>124</v>
+        <v>161</v>
       </c>
       <c r="C26" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D26">
         <v>13</v>
       </c>
-      <c r="E26" t="s">
-        <v>158</v>
-      </c>
-      <c r="F26" t="s">
+      <c r="E26" s="19" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="F26" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -3990,7 +4016,7 @@
       </c>
       <c r="F27"/>
     </row>
-    <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -4005,7 +4031,7 @@
       </c>
       <c r="F28"/>
     </row>
-    <row r="29" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -4020,7 +4046,7 @@
       </c>
       <c r="F29"/>
     </row>
-    <row r="30" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -4035,7 +4061,7 @@
       </c>
       <c r="F30"/>
     </row>
-    <row r="31" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -4050,7 +4076,7 @@
       </c>
       <c r="F31"/>
     </row>
-    <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -4065,7 +4091,7 @@
       </c>
       <c r="F32"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -4080,7 +4106,7 @@
       </c>
       <c r="F33"/>
     </row>
-    <row r="34" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -4095,7 +4121,7 @@
       </c>
       <c r="F34"/>
     </row>
-    <row r="35" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -4110,7 +4136,7 @@
       </c>
       <c r="F35"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -4125,7 +4151,7 @@
       </c>
       <c r="F36"/>
     </row>
-    <row r="37" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>30</v>
       </c>
@@ -4140,7 +4166,7 @@
       </c>
       <c r="F37"/>
     </row>
-    <row r="38" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>30</v>
       </c>
@@ -4155,7 +4181,7 @@
       </c>
       <c r="F38"/>
     </row>
-    <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>30</v>
       </c>
@@ -4170,7 +4196,7 @@
       </c>
       <c r="F39"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>30</v>
       </c>
@@ -4185,7 +4211,7 @@
       </c>
       <c r="F40"/>
     </row>
-    <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>31</v>
       </c>
@@ -4200,9 +4226,7 @@
       </c>
       <c r="F41"/>
     </row>
-    <row r="42" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="F42"/>
-    </row>
+    <row r="42" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="43" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B43" s="7"/>
       <c r="F43"/>
@@ -4674,401 +4698,85 @@
       <c r="D16"/>
       <c r="F16"/>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C17"/>
-      <c r="D17"/>
-      <c r="F17"/>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C18"/>
-      <c r="D18"/>
-      <c r="F18"/>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C19"/>
-      <c r="D19"/>
-      <c r="F19"/>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C20"/>
-      <c r="D20"/>
-      <c r="F20"/>
-    </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C21"/>
-      <c r="D21"/>
-      <c r="F21"/>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C22"/>
-      <c r="D22"/>
-      <c r="F22"/>
-    </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C23"/>
-      <c r="D23"/>
-      <c r="F23"/>
-    </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C24"/>
-      <c r="D24"/>
-      <c r="F24"/>
-    </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C25"/>
-      <c r="D25"/>
-      <c r="F25"/>
-    </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C26"/>
-      <c r="D26"/>
-      <c r="F26"/>
-    </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C27"/>
-      <c r="D27"/>
-      <c r="F27"/>
-    </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C28"/>
-      <c r="D28"/>
-      <c r="F28"/>
-    </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C29"/>
-      <c r="D29"/>
-      <c r="F29"/>
-    </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C30"/>
-      <c r="D30"/>
-      <c r="F30"/>
-    </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C31"/>
-      <c r="D31"/>
-      <c r="F31"/>
-    </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C32"/>
-      <c r="D32"/>
-      <c r="F32"/>
-    </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C33"/>
-      <c r="D33"/>
-      <c r="F33"/>
-    </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C34"/>
-      <c r="D34"/>
-      <c r="F34"/>
-    </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C35"/>
-      <c r="D35"/>
-      <c r="F35"/>
-    </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C36"/>
-      <c r="D36"/>
-      <c r="F36"/>
-    </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C37"/>
-      <c r="D37"/>
-      <c r="F37"/>
-    </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C38"/>
-      <c r="D38"/>
-      <c r="F38"/>
-    </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C39"/>
-      <c r="D39"/>
-      <c r="F39"/>
-    </row>
-    <row r="40" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C40"/>
-      <c r="D40"/>
-      <c r="F40"/>
-    </row>
-    <row r="41" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C41"/>
-      <c r="D41"/>
-      <c r="F41"/>
-    </row>
-    <row r="42" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C42"/>
-      <c r="D42"/>
-      <c r="F42"/>
-    </row>
-    <row r="43" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C43"/>
-      <c r="D43"/>
-      <c r="F43"/>
-    </row>
-    <row r="44" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C44"/>
-      <c r="D44"/>
-      <c r="F44"/>
-    </row>
-    <row r="45" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C45"/>
-      <c r="D45"/>
-      <c r="F45"/>
-    </row>
-    <row r="46" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C46"/>
-      <c r="D46"/>
-      <c r="F46"/>
-    </row>
-    <row r="47" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C47"/>
-      <c r="D47"/>
-      <c r="F47"/>
-    </row>
-    <row r="48" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C48"/>
-      <c r="D48"/>
-      <c r="F48"/>
-    </row>
-    <row r="49" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C49"/>
-      <c r="D49"/>
-      <c r="F49"/>
-    </row>
-    <row r="50" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C50"/>
-      <c r="D50"/>
-      <c r="F50"/>
-    </row>
-    <row r="51" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C51"/>
-      <c r="D51"/>
-      <c r="F51"/>
-    </row>
-    <row r="52" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C52"/>
-      <c r="D52"/>
-      <c r="F52"/>
-    </row>
-    <row r="53" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C53"/>
-      <c r="D53"/>
-      <c r="F53"/>
-    </row>
-    <row r="54" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C54"/>
-      <c r="D54"/>
-      <c r="F54"/>
-    </row>
-    <row r="55" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C55"/>
-      <c r="D55"/>
-      <c r="F55"/>
-    </row>
-    <row r="56" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C56"/>
-      <c r="D56"/>
-      <c r="F56"/>
-    </row>
-    <row r="57" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C57"/>
-      <c r="D57"/>
-      <c r="F57"/>
-    </row>
-    <row r="58" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C58"/>
-      <c r="D58"/>
-      <c r="F58"/>
-    </row>
-    <row r="59" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C59"/>
-      <c r="D59"/>
-      <c r="F59"/>
-    </row>
-    <row r="60" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C60"/>
-      <c r="D60"/>
-      <c r="F60"/>
-    </row>
-    <row r="61" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C61"/>
-      <c r="D61"/>
-      <c r="F61"/>
-    </row>
-    <row r="62" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C62"/>
-      <c r="D62"/>
-      <c r="F62"/>
-    </row>
-    <row r="63" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C63"/>
-      <c r="D63"/>
-      <c r="F63"/>
-    </row>
-    <row r="64" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C64"/>
-      <c r="D64"/>
-      <c r="F64"/>
-    </row>
-    <row r="65" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C65"/>
-      <c r="D65"/>
-      <c r="F65"/>
-    </row>
-    <row r="66" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C66"/>
-      <c r="D66"/>
-      <c r="F66"/>
-    </row>
-    <row r="67" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C67"/>
-      <c r="D67"/>
-      <c r="F67"/>
-    </row>
-    <row r="68" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C68"/>
-      <c r="D68"/>
-      <c r="F68"/>
-    </row>
-    <row r="69" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C69"/>
-      <c r="D69"/>
-      <c r="F69"/>
-    </row>
-    <row r="70" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C70"/>
-      <c r="D70"/>
-      <c r="F70"/>
-    </row>
-    <row r="71" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C71"/>
-      <c r="D71"/>
-      <c r="F71"/>
-    </row>
-    <row r="72" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C72"/>
-      <c r="D72"/>
-      <c r="F72"/>
-    </row>
-    <row r="73" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C73"/>
-      <c r="D73"/>
-      <c r="F73"/>
-    </row>
-    <row r="74" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C74"/>
-      <c r="D74"/>
-      <c r="F74"/>
-    </row>
-    <row r="75" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C75"/>
-      <c r="D75"/>
-      <c r="F75"/>
-    </row>
-    <row r="76" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C76"/>
-      <c r="D76"/>
-      <c r="F76"/>
-    </row>
-    <row r="77" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C77"/>
-      <c r="D77"/>
-      <c r="F77"/>
-    </row>
-    <row r="78" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C78"/>
-      <c r="D78"/>
-      <c r="F78"/>
-    </row>
-    <row r="79" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C79"/>
-      <c r="D79"/>
-      <c r="F79"/>
-    </row>
-    <row r="80" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C80"/>
-      <c r="D80"/>
-      <c r="F80"/>
-    </row>
-    <row r="81" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C81"/>
-      <c r="D81"/>
-      <c r="F81"/>
-    </row>
-    <row r="82" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C82"/>
-      <c r="D82"/>
-      <c r="F82"/>
-    </row>
-    <row r="83" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C83"/>
-      <c r="D83"/>
-      <c r="F83"/>
-    </row>
-    <row r="84" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C84"/>
-      <c r="D84"/>
-      <c r="F84"/>
-    </row>
-    <row r="85" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C85"/>
-      <c r="D85"/>
-      <c r="F85"/>
-    </row>
-    <row r="86" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C86"/>
-      <c r="D86"/>
-      <c r="F86"/>
-    </row>
-    <row r="87" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C87"/>
-      <c r="D87"/>
-      <c r="F87"/>
-    </row>
-    <row r="88" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C88"/>
-      <c r="D88"/>
-      <c r="F88"/>
-    </row>
-    <row r="89" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C89"/>
-      <c r="D89"/>
-      <c r="F89"/>
-    </row>
-    <row r="90" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C90"/>
-      <c r="D90"/>
-      <c r="F90"/>
-    </row>
-    <row r="91" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C91"/>
-      <c r="D91"/>
-      <c r="F91"/>
-    </row>
-    <row r="92" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C92"/>
-      <c r="D92"/>
-      <c r="F92"/>
-    </row>
-    <row r="93" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C93"/>
-      <c r="D93"/>
-      <c r="F93"/>
-    </row>
-    <row r="94" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C94"/>
-      <c r="D94"/>
-      <c r="F94"/>
-    </row>
-    <row r="95" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C95"/>
-      <c r="D95"/>
-      <c r="F95"/>
-    </row>
+    <row r="17" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="18" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="19" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="20" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="21" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="22" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="23" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="24" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="25" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="26" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="27" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="28" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="29" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="30" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="31" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="32" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="33" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="34" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="35" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="36" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="37" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="38" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="39" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="40" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="41" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="42" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="43" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="44" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="45" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="46" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="47" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="48" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="49" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="50" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="51" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="52" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="53" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="54" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="55" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="56" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="57" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="58" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="59" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="60" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="61" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="62" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="63" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="64" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="65" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="66" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="67" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="68" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="69" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="70" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="71" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="72" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="73" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="74" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="75" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="76" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="77" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="78" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="79" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="80" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="81" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="82" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="83" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="84" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="85" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="86" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="87" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="88" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="89" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="90" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="91" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="92" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="93" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="94" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="95" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactoring: moving SelenideElements to the top of page objects
</commit_message>
<xml_diff>
--- a/sharelane_checklist.xlsx
+++ b/sharelane_checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Test Automation\Java\hw4_Sharelane\hw4_sharelane\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4C34E5C-DFEC-48B3-808E-4ADCFC74BEFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3926A202-9A76-4E12-8C4B-E5655C359401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="Требования" sheetId="4" r:id="rId1"/>
     <sheet name="Тест-кейсы и приоретизация" sheetId="1" r:id="rId2"/>
     <sheet name="Тест-кейсы на автоматизацию" sheetId="5" r:id="rId3"/>
-    <sheet name="Тест-кейсы по багам и фичам" sheetId="3" r:id="rId4"/>
-    <sheet name="Фиксы" sheetId="2" r:id="rId5"/>
+    <sheet name="Фиксы" sheetId="2" r:id="rId4"/>
+    <sheet name="Тест-кейсы по багам и фичам" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="175">
   <si>
     <t>Статус</t>
   </si>
@@ -545,6 +545,27 @@
   </si>
   <si>
     <t>Проверить что кнопка Proceed to Checkout ведёт на страницу Checkout</t>
+  </si>
+  <si>
+    <t>1. Выдержать единый стиль для всех пейдж обжектов (элементы как поля, в методах локаторы не храним)</t>
+  </si>
+  <si>
+    <t>2. убрать абсолютные локаторы и сделать локаторы максимально стабильными и лаконичными</t>
+  </si>
+  <si>
+    <t>3. Для методов которые работают с данными и параметрами постараться использовал модели (юзер билдер, ломбок) использовать фейкер для генерации случайных данных</t>
+  </si>
+  <si>
+    <t>4. все общие данные базовый урл, время ожидание и прочее вынести в проперти ридер и реализовать сам проперти ридер</t>
+  </si>
+  <si>
+    <t>5. Для работы с джсонами реализовать джс утилити класс который будет вычитывать джсон и возвращать нужный обьект либо коллекцию обьектов</t>
+  </si>
+  <si>
+    <t>6. выдержать структуры проекта (тесты, бизнесс обьекты, кор(утилиты хелперы))</t>
+  </si>
+  <si>
+    <t>7. разнести класс шеирлен утилити на отдельные классы (либо методы в пейдж обжекты либо в класс степов)</t>
   </si>
 </sst>
 </file>
@@ -856,13 +877,7 @@
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6998AABF-FC77-48A5-8AA0-30BE1579D29E}" name="Table13" displayName="Table13" ref="A1:F41" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2">
-  <autoFilter ref="A1:F41" xr:uid="{FE89EFD3-F5E6-427A-A4AE-782233C9841D}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="Делаем"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:F41" xr:uid="{FE89EFD3-F5E6-427A-A4AE-782233C9841D}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F41">
     <sortCondition descending="1" ref="D1:D41"/>
   </sortState>
@@ -1852,7 +1867,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J123"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -3509,9 +3524,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B755BA-AB1D-4BD0-B742-796615240701}">
   <dimension ref="A1:F123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -3543,7 +3556,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -3563,7 +3576,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -3697,7 +3710,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -3714,7 +3727,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -3731,7 +3744,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -3748,7 +3761,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -3765,7 +3778,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -3783,7 +3796,7 @@
       </c>
       <c r="F14"/>
     </row>
-    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -3801,7 +3814,7 @@
       </c>
       <c r="F15"/>
     </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -3819,7 +3832,7 @@
       </c>
       <c r="F16"/>
     </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -3837,7 +3850,7 @@
       </c>
       <c r="F17"/>
     </row>
-    <row r="18" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -3855,7 +3868,7 @@
       </c>
       <c r="F18"/>
     </row>
-    <row r="19" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -3891,7 +3904,7 @@
       </c>
       <c r="F20"/>
     </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -3909,7 +3922,7 @@
       </c>
       <c r="F21"/>
     </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -3945,7 +3958,7 @@
       </c>
       <c r="F23"/>
     </row>
-    <row r="24" spans="1:6" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -3963,7 +3976,7 @@
       </c>
       <c r="F24"/>
     </row>
-    <row r="25" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -3981,7 +3994,7 @@
       </c>
       <c r="F25"/>
     </row>
-    <row r="26" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -4001,7 +4014,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -4016,7 +4029,7 @@
       </c>
       <c r="F27"/>
     </row>
-    <row r="28" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -4031,7 +4044,7 @@
       </c>
       <c r="F28"/>
     </row>
-    <row r="29" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -4046,7 +4059,7 @@
       </c>
       <c r="F29"/>
     </row>
-    <row r="30" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -4061,7 +4074,7 @@
       </c>
       <c r="F30"/>
     </row>
-    <row r="31" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -4076,7 +4089,7 @@
       </c>
       <c r="F31"/>
     </row>
-    <row r="32" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -4091,7 +4104,7 @@
       </c>
       <c r="F32"/>
     </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -4106,7 +4119,7 @@
       </c>
       <c r="F33"/>
     </row>
-    <row r="34" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -4121,7 +4134,7 @@
       </c>
       <c r="F34"/>
     </row>
-    <row r="35" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -4136,7 +4149,7 @@
       </c>
       <c r="F35"/>
     </row>
-    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -4151,7 +4164,7 @@
       </c>
       <c r="F36"/>
     </row>
-    <row r="37" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>30</v>
       </c>
@@ -4166,7 +4179,7 @@
       </c>
       <c r="F37"/>
     </row>
-    <row r="38" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>30</v>
       </c>
@@ -4181,7 +4194,7 @@
       </c>
       <c r="F38"/>
     </row>
-    <row r="39" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>30</v>
       </c>
@@ -4196,7 +4209,7 @@
       </c>
       <c r="F39"/>
     </row>
-    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>30</v>
       </c>
@@ -4211,7 +4224,7 @@
       </c>
       <c r="F40"/>
     </row>
-    <row r="41" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>31</v>
       </c>
@@ -4587,6 +4600,76 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55D8DF8D-3BDE-4455-81F1-A528355B1E3F}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="3.90625" customWidth="1"/>
+    <col min="2" max="2" width="66.08984375" customWidth="1"/>
+    <col min="3" max="3" width="16.54296875" customWidth="1"/>
+    <col min="4" max="4" width="59.6328125" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="B2" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="B3" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B4" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="B5" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="B7" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="B8" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE367AB7-4F21-4DFE-882A-DED052437329}">
   <dimension ref="A1:F95"/>
   <sheetViews>
@@ -4780,42 +4863,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55D8DF8D-3BDE-4455-81F1-A528355B1E3F}">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="A1:D1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="3.90625" customWidth="1"/>
-    <col min="2" max="2" width="66.08984375" customWidth="1"/>
-    <col min="3" max="3" width="16.54296875" customWidth="1"/>
-    <col min="4" max="4" width="59.6328125" style="3" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B4" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>